<commit_message>
Testing the time execution of these codes
</commit_message>
<xml_diff>
--- a/files/Rev00_DataGraphics_PTBR.xlsx
+++ b/files/Rev00_DataGraphics_PTBR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/19e359efc7a6f442/Desktop/Enari/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AECF5A1F-C523-497A-B2A1-66620ACB315E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="8_{AECF5A1F-C523-497A-B2A1-66620ACB315E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45BFA939-BA54-47EC-9CAD-54ADEC3FF40F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="8" activeTab="8" xr2:uid="{17A1DBDD-B353-481C-9E41-6E9A6A8B360B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{17A1DBDD-B353-481C-9E41-6E9A6A8B360B}"/>
   </bookViews>
   <sheets>
     <sheet name="Teste" sheetId="1" state="hidden" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="14">
   <si>
     <t>Algoritmo</t>
   </si>
@@ -86,6 +86,9 @@
   <si>
     <t>CoutingSort</t>
   </si>
+  <si>
+    <t>RadixSort</t>
+  </si>
 </sst>
 </file>
 
@@ -100,12 +103,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -120,13 +129,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2442,17 +2465,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Ordenados!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>BubbleSort</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:ln w="22225" cap="rnd">
               <a:solidFill>
@@ -2508,6 +2520,21 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.0309999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0690000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.1830000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0179999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0109999999999998E-3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2521,17 +2548,6 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Ordenados!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>InsertionSort</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:ln w="22225" cap="rnd">
               <a:solidFill>
@@ -2600,17 +2616,6 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Ordenados!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>SelectionSort</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:ln w="22225" cap="rnd">
               <a:solidFill>
@@ -2679,17 +2684,6 @@
         <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Ordenados!$E$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>MergeSort</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:ln w="22225" cap="rnd">
               <a:solidFill>
@@ -2756,17 +2750,6 @@
         <c:ser>
           <c:idx val="4"/>
           <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Ordenados!$F$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>QuickSort</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:ln w="22225" cap="rnd">
               <a:solidFill>
@@ -2833,17 +2816,6 @@
         <c:ser>
           <c:idx val="5"/>
           <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Ordenados!$G$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>HeapSort</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:ln w="22225" cap="rnd">
               <a:solidFill>
@@ -2912,17 +2884,6 @@
         <c:ser>
           <c:idx val="6"/>
           <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Ordenados!$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>CoutingSort</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:ln w="22225" cap="rnd">
               <a:solidFill>
@@ -3359,6 +3320,21 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.32450000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3774</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.81595</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22.1435</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35.180549999999997</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3434,10 +3410,25 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'!Ordenados'!$C$2:$C$6</c:f>
+              <c:f>'!Ordenados'!$E$2:$E$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>7.1536666666666667E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1510000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.7834000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.7357333333333338E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.0836999999999997E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3590,10 +3581,13 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'!Ordenados'!$E$2:$E$6</c:f>
+              <c:f>'!Ordenados'!#REF!</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3769,7 +3763,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>CoutingSort</c:v>
+                  <c:v>RadixSort</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3827,7 +3821,91 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'!Ordenados'!$H$2:$H$6</c:f>
+              <c:f>'!Ordenados'!$H$3:$H$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="3">
+                  <c:v>2.2390333333333332E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-1D8A-4CD0-96CD-74A059675AAF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'!Ordenados'!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CoutingSort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="plus"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'!Ordenados'!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'!Ordenados'!$I$2:$I$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3837,7 +3915,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-1D8A-4CD0-96CD-74A059675AAF}"/>
+              <c16:uniqueId val="{00000000-05DA-469E-93E4-09C6FFDC7826}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -15462,7 +15540,7 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>137160</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>83820</xdr:rowOff>
     </xdr:from>
@@ -15502,15 +15580,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>91440</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>525780</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>548640</xdr:colOff>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -15843,7 +15921,7 @@
   <autoFilter ref="A1:H6" xr:uid="{A40AA6AD-2F47-43F1-B765-C68DAECD3079}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{7BB7217C-59F8-4792-9EA0-0720D6D8B12E}" name="Tamanho"/>
-    <tableColumn id="2" xr3:uid="{C5127529-A4E4-4639-A4FA-738598E99596}" name="BubbleSort"/>
+    <tableColumn id="2" xr3:uid="{C5127529-A4E4-4639-A4FA-738598E99596}" name="BubbleSort" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{D3407327-A185-4351-A55C-14014B1B867D}" name="InsertionSort"/>
     <tableColumn id="4" xr3:uid="{85C71698-96C8-48BF-9E4F-A31F4588E93A}" name="SelectionSort"/>
     <tableColumn id="5" xr3:uid="{D89F0557-14DD-46AD-9565-6B8B49785A1D}" name="MergeSort"/>
@@ -15856,16 +15934,17 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{8E4EE357-D0C4-43BC-B881-53E1F8B229C0}" name="ValoresInversamenteOrdenados" displayName="ValoresInversamenteOrdenados" ref="A1:H6" totalsRowShown="0">
-  <autoFilter ref="A1:H6" xr:uid="{8E4EE357-D0C4-43BC-B881-53E1F8B229C0}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{8E4EE357-D0C4-43BC-B881-53E1F8B229C0}" name="ValoresInversamenteOrdenados" displayName="ValoresInversamenteOrdenados" ref="A1:I6" totalsRowShown="0">
+  <autoFilter ref="A1:I6" xr:uid="{8E4EE357-D0C4-43BC-B881-53E1F8B229C0}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{C1F8DEBA-C1C8-4F0D-B5A8-25CE5185E617}" name="Tamanho"/>
     <tableColumn id="2" xr3:uid="{73836CB1-A1D9-4D27-AA51-8096EC2B23FB}" name="BubbleSort"/>
-    <tableColumn id="3" xr3:uid="{50D01E1E-E49D-48B8-9D64-68BB18FD132D}" name="InsertionSort"/>
+    <tableColumn id="3" xr3:uid="{50D01E1E-E49D-48B8-9D64-68BB18FD132D}" name="InsertionSort" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{BF3C1C79-92F0-4E93-AE3F-44D10600C26D}" name="SelectionSort"/>
     <tableColumn id="5" xr3:uid="{71DF7DE3-1D14-438B-AA85-26258AB0E16E}" name="MergeSort"/>
     <tableColumn id="6" xr3:uid="{D7044A8A-343F-410A-A47C-299C79374E83}" name="QuickSort"/>
     <tableColumn id="7" xr3:uid="{44EE4653-5828-4AD8-89F5-DCD6FFFB7171}" name="HeapSort"/>
+    <tableColumn id="9" xr3:uid="{06AF528E-0B37-497F-86E3-9CA2A978E533}" name="RadixSort"/>
     <tableColumn id="8" xr3:uid="{1AF9EE2E-6E80-48E6-A0EA-B411C6533961}" name="CoutingSort"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -16641,7 +16720,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16686,25 +16765,41 @@
       <c r="A2">
         <v>10000</v>
       </c>
+      <c r="B2" s="1">
+        <v>2.0309999999999998E-3</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>20000</v>
       </c>
+      <c r="B3" s="1">
+        <v>3.0690000000000001E-3</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>40000</v>
       </c>
+      <c r="B4" s="1">
+        <v>5.1830000000000001E-3</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>80000</v>
       </c>
+      <c r="B5" s="1">
+        <v>2.0179999999999998E-3</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>100000</v>
+      </c>
+      <c r="B6" s="1">
+        <f>(0.002015+0.002007)/2</f>
+        <v>2.0109999999999998E-3</v>
       </c>
     </row>
   </sheetData>
@@ -16721,10 +16816,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16732,13 +16827,14 @@
     <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" customWidth="1"/>
+    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -16761,32 +16857,84 @@
         <v>11</v>
       </c>
       <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10000</v>
       </c>
+      <c r="B2">
+        <v>0.32450000000000001</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="E2">
+        <f>(0.006058 + 0.006755 + 0.008648)/3</f>
+        <v>7.1536666666666667E-3</v>
+      </c>
+      <c r="H2">
+        <f>(0.004854+0.005872+0.005069)/3</f>
+        <v>5.2649999999999997E-3</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>20000</v>
       </c>
+      <c r="B3">
+        <v>1.3774</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="E3">
+        <f>(0.032114 + 0.017049 + 0.015367)/3</f>
+        <v>2.1510000000000001E-2</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>40000</v>
       </c>
+      <c r="B4">
+        <v>5.81595</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="E4">
+        <f>(0.025146 + 0.031812 + 0.026544)/3</f>
+        <v>2.7834000000000001E-2</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>80000</v>
       </c>
+      <c r="B5">
+        <v>22.1435</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="E5">
+        <f>(0.077793 + 0.082077 + 0.042202)/3</f>
+        <v>6.7357333333333338E-2</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>100000</v>
+      </c>
+      <c r="B6">
+        <f>(36.2484 + 34.1127)/2</f>
+        <v>35.180549999999997</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="E6">
+        <f>(0.081262 + 0.065537 + 0.065712)/3</f>
+        <v>7.0836999999999997E-2</v>
+      </c>
+      <c r="H6">
+        <f>(0.022816 + 0.024383 + 0.019972)/3</f>
+        <v>2.2390333333333332E-2</v>
       </c>
     </row>
   </sheetData>
@@ -16806,7 +16954,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H6"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17220,7 +17368,7 @@
   </sheetPr>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
General rev on the code.
</commit_message>
<xml_diff>
--- a/files/Rev00_DataGraphics_PTBR.xlsx
+++ b/files/Rev00_DataGraphics_PTBR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/19e359efc7a6f442/Desktop/Enari/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="73" documentId="8_{AECF5A1F-C523-497A-B2A1-66620ACB315E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBEE1BD3-C1B4-4DE8-BB95-C06671E9DB6D}"/>
+  <xr:revisionPtr revIDLastSave="143" documentId="8_{AECF5A1F-C523-497A-B2A1-66620ACB315E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB45B3A0-A7EB-467F-833C-C7BBEC07D751}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{17A1DBDD-B353-481C-9E41-6E9A6A8B360B}"/>
   </bookViews>
@@ -94,6 +94,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="170" formatCode="0.0000"/>
+    <numFmt numFmtId="171" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -129,16 +133,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="171" formatCode="0.000"/>
     </dxf>
     <dxf>
       <fill>
@@ -3317,22 +3330,22 @@
             <c:numRef>
               <c:f>'!Ordenados'!$B$2:$B$6</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.32450000000000001</c:v>
+                  <c:v>0.37533833333333333</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3774</c:v>
+                  <c:v>1.5142666666666669</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.81595</c:v>
+                  <c:v>5.6746633333333323</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22.1435</c:v>
+                  <c:v>22.592433333333332</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35.180549999999997</c:v>
+                  <c:v>35.15826666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3340,7 +3353,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1D8A-4CD0-96CD-74A059675AAF}"/>
+              <c16:uniqueId val="{00000000-BA95-4431-A92C-89FE8916D0CD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3409,24 +3422,12 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'!Ordenados'!$E$2:$E$6</c:f>
+              <c:f>'!Ordenados'!$C$2:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>7.1536666666666667E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.1510000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.7834000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.7357333333333338E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.0836999999999997E-2</c:v>
+                <c:pt idx="4" formatCode="0.00">
+                  <c:v>29.435566666666663</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3434,7 +3435,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-1D8A-4CD0-96CD-74A059675AAF}"/>
+              <c16:uniqueId val="{00000001-BA95-4431-A92C-89FE8916D0CD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3513,7 +3514,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-1D8A-4CD0-96CD-74A059675AAF}"/>
+              <c16:uniqueId val="{00000002-BA95-4431-A92C-89FE8916D0CD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3541,10 +3542,12 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="x"/>
+            <c:symbol val="square"/>
             <c:size val="6"/>
             <c:spPr>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
                   <a:schemeClr val="accent4"/>
@@ -3580,12 +3583,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'!Ordenados'!#REF!</c:f>
+              <c:f>'!Ordenados'!$E$2:$E$6</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>7.1536666666666667E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1510000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.7834000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.7357333333333338E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.0836999999999997E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3593,7 +3608,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-1D8A-4CD0-96CD-74A059675AAF}"/>
+              <c16:uniqueId val="{00000003-BA95-4431-A92C-89FE8916D0CD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3621,7 +3636,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="star"/>
+            <c:symbol val="x"/>
             <c:size val="6"/>
             <c:spPr>
               <a:noFill/>
@@ -3670,7 +3685,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-1D8A-4CD0-96CD-74A059675AAF}"/>
+              <c16:uniqueId val="{00000004-BA95-4431-A92C-89FE8916D0CD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3749,7 +3764,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-1D8A-4CD0-96CD-74A059675AAF}"/>
+              <c16:uniqueId val="{00000005-BA95-4431-A92C-89FE8916D0CD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3820,20 +3835,23 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'!Ordenados'!$H$3:$H$6</c:f>
+              <c:f>'!Ordenados'!$H$2:$H$6</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>5.2649999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>6.1253333333333333E-3</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>1.4749333333333335E-2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>2.0516000000000003E-2</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>2.3499999999999997E-2</c:v>
                 </c:pt>
               </c:numCache>
@@ -3842,7 +3860,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-1D8A-4CD0-96CD-74A059675AAF}"/>
+              <c16:uniqueId val="{00000006-BA95-4431-A92C-89FE8916D0CD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3923,7 +3941,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-05DA-469E-93E4-09C6FFDC7826}"/>
+              <c16:uniqueId val="{00000007-BA95-4431-A92C-89FE8916D0CD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4021,7 +4039,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -15596,8 +15614,8 @@
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>548640</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15933,7 +15951,7 @@
   <autoFilter ref="A1:H6" xr:uid="{A40AA6AD-2F47-43F1-B765-C68DAECD3079}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{7BB7217C-59F8-4792-9EA0-0720D6D8B12E}" name="Tamanho"/>
-    <tableColumn id="2" xr3:uid="{C5127529-A4E4-4639-A4FA-738598E99596}" name="BubbleSort" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{C5127529-A4E4-4639-A4FA-738598E99596}" name="BubbleSort" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{D3407327-A185-4351-A55C-14014B1B867D}" name="InsertionSort"/>
     <tableColumn id="4" xr3:uid="{85C71698-96C8-48BF-9E4F-A31F4588E93A}" name="SelectionSort"/>
     <tableColumn id="5" xr3:uid="{D89F0557-14DD-46AD-9565-6B8B49785A1D}" name="MergeSort"/>
@@ -15953,10 +15971,10 @@
     <tableColumn id="2" xr3:uid="{73836CB1-A1D9-4D27-AA51-8096EC2B23FB}" name="BubbleSort"/>
     <tableColumn id="3" xr3:uid="{50D01E1E-E49D-48B8-9D64-68BB18FD132D}" name="InsertionSort" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{BF3C1C79-92F0-4E93-AE3F-44D10600C26D}" name="SelectionSort"/>
-    <tableColumn id="5" xr3:uid="{71DF7DE3-1D14-438B-AA85-26258AB0E16E}" name="MergeSort"/>
+    <tableColumn id="5" xr3:uid="{71DF7DE3-1D14-438B-AA85-26258AB0E16E}" name="MergeSort" dataDxfId="2"/>
     <tableColumn id="6" xr3:uid="{D7044A8A-343F-410A-A47C-299C79374E83}" name="QuickSort"/>
     <tableColumn id="7" xr3:uid="{44EE4653-5828-4AD8-89F5-DCD6FFFB7171}" name="HeapSort"/>
-    <tableColumn id="9" xr3:uid="{06AF528E-0B37-497F-86E3-9CA2A978E533}" name="RadixSort"/>
+    <tableColumn id="9" xr3:uid="{06AF528E-0B37-497F-86E3-9CA2A978E533}" name="RadixSort" dataDxfId="1"/>
     <tableColumn id="8" xr3:uid="{1AF9EE2E-6E80-48E6-A0EA-B411C6533961}" name="CoutingSort"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -16831,18 +16849,19 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -16879,14 +16898,15 @@
       <c r="A2">
         <v>10000</v>
       </c>
-      <c r="B2">
-        <v>0.32450000000000001</v>
-      </c>
-      <c r="E2">
+      <c r="B2" s="4">
+        <f>(0.400121 + 0.35489 + 0.371004)/3</f>
+        <v>0.37533833333333333</v>
+      </c>
+      <c r="E2" s="3">
         <f>(0.006058 + 0.006755 + 0.008648)/3</f>
         <v>7.1536666666666667E-3</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="2">
         <f>(0.004854+0.005872+0.005069)/3</f>
         <v>5.2649999999999997E-3</v>
       </c>
@@ -16895,14 +16915,15 @@
       <c r="A3">
         <v>20000</v>
       </c>
-      <c r="B3">
-        <v>1.3774</v>
-      </c>
-      <c r="E3">
+      <c r="B3" s="4">
+        <f>(1.59393+1.47473+1.47414)/3</f>
+        <v>1.5142666666666669</v>
+      </c>
+      <c r="E3" s="3">
         <f>(0.032114 + 0.017049 + 0.015367)/3</f>
         <v>2.1510000000000001E-2</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="2">
         <f>(0.005196+0.005353+0.007827)/3</f>
         <v>6.1253333333333333E-3</v>
       </c>
@@ -16911,14 +16932,15 @@
       <c r="A4">
         <v>40000</v>
       </c>
-      <c r="B4">
-        <v>5.81595</v>
-      </c>
-      <c r="E4">
+      <c r="B4" s="4">
+        <f>(5.73225 + 5.69743 + 5.59431)/3</f>
+        <v>5.6746633333333323</v>
+      </c>
+      <c r="E4" s="3">
         <f>(0.025146 + 0.031812 + 0.026544)/3</f>
         <v>2.7834000000000001E-2</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="2">
         <f>(0.015147+0.012408+0.016693)/3</f>
         <v>1.4749333333333335E-2</v>
       </c>
@@ -16927,14 +16949,15 @@
       <c r="A5">
         <v>80000</v>
       </c>
-      <c r="B5">
-        <v>22.1435</v>
-      </c>
-      <c r="E5">
+      <c r="B5" s="4">
+        <f>(22.6429+22.6126+22.5218)/3</f>
+        <v>22.592433333333332</v>
+      </c>
+      <c r="E5" s="3">
         <f>(0.077793 + 0.082077 + 0.042202)/3</f>
         <v>6.7357333333333338E-2</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="2">
         <f>(0.020408+0.022819+0.018321)/3</f>
         <v>2.0516000000000003E-2</v>
       </c>
@@ -16943,15 +16966,19 @@
       <c r="A6">
         <v>100000</v>
       </c>
-      <c r="B6">
-        <f>(36.2484 + 34.1127)/2</f>
-        <v>35.180549999999997</v>
-      </c>
-      <c r="E6">
+      <c r="B6" s="4">
+        <f>(35.2107+35.4054+34.8587)/3</f>
+        <v>35.15826666666667</v>
+      </c>
+      <c r="C6" s="4">
+        <f>(29.7728+28.9981+29.5358)/3</f>
+        <v>29.435566666666663</v>
+      </c>
+      <c r="E6" s="3">
         <f>(0.081262 + 0.065537 + 0.065712)/3</f>
         <v>7.0836999999999997E-2</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="2">
         <f>(0.022816 + 0.024383 + 0.023301)/3</f>
         <v>2.3499999999999997E-2</v>
       </c>

</xml_diff>

<commit_message>
Updated the datagraphics with new values
</commit_message>
<xml_diff>
--- a/files/Rev00_DataGraphics_PTBR.xlsx
+++ b/files/Rev00_DataGraphics_PTBR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/19e359efc7a6f442/Desktop/Enari/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="177" documentId="8_{AECF5A1F-C523-497A-B2A1-66620ACB315E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AEC8B137-F832-4A03-854D-3877CC5A827C}"/>
+  <xr:revisionPtr revIDLastSave="209" documentId="8_{AECF5A1F-C523-497A-B2A1-66620ACB315E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3BC54F2-FC0E-4FF7-BB6C-13F21CC07432}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{17A1DBDD-B353-481C-9E41-6E9A6A8B360B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="3" xr2:uid="{17A1DBDD-B353-481C-9E41-6E9A6A8B360B}"/>
   </bookViews>
   <sheets>
     <sheet name="Teste" sheetId="1" state="hidden" r:id="rId1"/>
@@ -4421,8 +4421,23 @@
             <c:numRef>
               <c:f>Aleatório!$C$2:$C$6</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.13780733333333331</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.61377533333333334</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2894266666666669</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>9.24057</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>14.346200000000001</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -16878,7 +16893,7 @@
   </sheetPr>
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -17045,15 +17060,15 @@
   </sheetPr>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
@@ -17095,6 +17110,10 @@
         <f>(0.325188+0.367946+0.316995)/3</f>
         <v>0.33670966666666668</v>
       </c>
+      <c r="C2" s="2">
+        <f>(0.133132+0.138554+0.141736)/3</f>
+        <v>0.13780733333333331</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -17104,6 +17123,10 @@
         <f>(1.52425+1.63456+1.52828)/3</f>
         <v>1.5623633333333331</v>
       </c>
+      <c r="C3" s="2">
+        <f>(0.547077+0.553206+0.741043)/3</f>
+        <v>0.61377533333333334</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -17113,6 +17136,10 @@
         <f>(5.53739+5.55585+5.68751)/3</f>
         <v>5.593583333333334</v>
       </c>
+      <c r="C4" s="2">
+        <f>(2.27114+2.26733+2.32981)/3</f>
+        <v>2.2894266666666669</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -17122,6 +17149,10 @@
         <f>(22.768+22.2722+22.102)/3</f>
         <v>22.380733333333335</v>
       </c>
+      <c r="C5">
+        <f>(9.1501+9.11789+9.45372)/3</f>
+        <v>9.24057</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -17130,6 +17161,10 @@
       <c r="B6" s="4">
         <f>(34.6919+35.3491+37.6816)/3</f>
         <v>35.907533333333333</v>
+      </c>
+      <c r="C6">
+        <f>(14.2188+14.4099+14.4099)/3</f>
+        <v>14.346200000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New update on the data graphics
</commit_message>
<xml_diff>
--- a/files/Rev00_DataGraphics_PTBR.xlsx
+++ b/files/Rev00_DataGraphics_PTBR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/19e359efc7a6f442/Desktop/Enari/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="379" documentId="8_{AECF5A1F-C523-497A-B2A1-66620ACB315E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5474F7F-7D64-419B-ADF1-82071934F2C0}"/>
+  <xr:revisionPtr revIDLastSave="388" documentId="8_{AECF5A1F-C523-497A-B2A1-66620ACB315E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1477AA46-2FAA-4F8F-A6EC-41BB7A1D21A8}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="3" xr2:uid="{17A1DBDD-B353-481C-9E41-6E9A6A8B360B}"/>
   </bookViews>
@@ -134,9 +134,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="167" formatCode="0.000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -186,19 +187,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="11">
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.000000"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.00000"/>
@@ -207,22 +227,7 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="0.00000"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.00000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.00000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0000"/>
     </dxf>
     <dxf>
       <fill>
@@ -4186,8 +4191,14 @@
             <c:numRef>
               <c:f>'!Ordenados'!$G$2:$G$6</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.4443333333333335E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.5646666666666665E-3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -16995,7 +17006,7 @@
   <autoFilter ref="A1:I6" xr:uid="{A40AA6AD-2F47-43F1-B765-C68DAECD3079}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{7BB7217C-59F8-4792-9EA0-0720D6D8B12E}" name="Tamanho"/>
-    <tableColumn id="2" xr3:uid="{C5127529-A4E4-4639-A4FA-738598E99596}" name="BubbleSort" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{C5127529-A4E4-4639-A4FA-738598E99596}" name="BubbleSort" dataDxfId="10"/>
     <tableColumn id="3" xr3:uid="{D3407327-A185-4351-A55C-14014B1B867D}" name="InsertionSort"/>
     <tableColumn id="4" xr3:uid="{85C71698-96C8-48BF-9E4F-A31F4588E93A}" name="SelectionSort"/>
     <tableColumn id="5" xr3:uid="{D89F0557-14DD-46AD-9565-6B8B49785A1D}" name="MergeSort"/>
@@ -17014,12 +17025,12 @@
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{C1F8DEBA-C1C8-4F0D-B5A8-25CE5185E617}" name="Tamanho"/>
     <tableColumn id="2" xr3:uid="{73836CB1-A1D9-4D27-AA51-8096EC2B23FB}" name="BubbleSort"/>
-    <tableColumn id="3" xr3:uid="{50D01E1E-E49D-48B8-9D64-68BB18FD132D}" name="InsertionSort" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{BF3C1C79-92F0-4E93-AE3F-44D10600C26D}" name="SelectionSort" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{71DF7DE3-1D14-438B-AA85-26258AB0E16E}" name="MergeSort" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{50D01E1E-E49D-48B8-9D64-68BB18FD132D}" name="InsertionSort" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{BF3C1C79-92F0-4E93-AE3F-44D10600C26D}" name="SelectionSort" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{71DF7DE3-1D14-438B-AA85-26258AB0E16E}" name="MergeSort" dataDxfId="7"/>
     <tableColumn id="6" xr3:uid="{D7044A8A-343F-410A-A47C-299C79374E83}" name="QuickSort"/>
-    <tableColumn id="7" xr3:uid="{44EE4653-5828-4AD8-89F5-DCD6FFFB7171}" name="HeapSort"/>
-    <tableColumn id="9" xr3:uid="{06AF528E-0B37-497F-86E3-9CA2A978E533}" name="RadixSort" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{44EE4653-5828-4AD8-89F5-DCD6FFFB7171}" name="HeapSort" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{06AF528E-0B37-497F-86E3-9CA2A978E533}" name="RadixSort" dataDxfId="1"/>
     <tableColumn id="8" xr3:uid="{1AF9EE2E-6E80-48E6-A0EA-B411C6533961}" name="CoutingSort"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -17031,14 +17042,14 @@
   <autoFilter ref="A1:I6" xr:uid="{59E19B13-715F-472A-A7B5-ACE0684BA986}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{88AB9604-3310-46A1-AD70-21C2608B01C8}" name="Tamanho"/>
-    <tableColumn id="2" xr3:uid="{AB29B0C4-1AC7-48FD-8D3C-13AA6916E031}" name="BubbleSort" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{AB29B0C4-1AC7-48FD-8D3C-13AA6916E031}" name="BubbleSort" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{277890D8-FE28-4EFB-A704-7CA343850008}" name="InsertionSort"/>
-    <tableColumn id="4" xr3:uid="{7B9C2A85-4991-44A3-8EB5-C25296FAD161}" name="SelectionSort" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{4450D16D-D01F-43DF-B8B1-9C2BAE2DFD58}" name="MergeSort" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{7B9C2A85-4991-44A3-8EB5-C25296FAD161}" name="SelectionSort" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{4450D16D-D01F-43DF-B8B1-9C2BAE2DFD58}" name="MergeSort" dataDxfId="4"/>
     <tableColumn id="6" xr3:uid="{8F5D90A6-8E0B-4E1B-8D02-4E5B09ACDCA0}" name="QuickSort"/>
     <tableColumn id="7" xr3:uid="{59D8846C-91B6-4237-BE54-A17E0A509527}" name="HeapSort"/>
-    <tableColumn id="8" xr3:uid="{6B8DE172-995E-41FE-BF4F-C27226F78BC4}" name="RadixSort" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{D222E4FB-3FC2-4727-958D-5584BD8905DB}" name="CoutingSort" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{6B8DE172-995E-41FE-BF4F-C27226F78BC4}" name="RadixSort" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{D222E4FB-3FC2-4727-958D-5584BD8905DB}" name="CoutingSort" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -17911,7 +17922,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17976,6 +17987,10 @@
         <f>(0.006058 + 0.006755 + 0.008648)/3</f>
         <v>7.1536666666666667E-3</v>
       </c>
+      <c r="G2" s="5">
+        <f>(0.002001+0.003001+0.002331)/3</f>
+        <v>2.4443333333333335E-3</v>
+      </c>
       <c r="H2" s="2">
         <f>(0.004854+0.005872+0.005069)/3</f>
         <v>5.2649999999999997E-3</v>
@@ -18004,6 +18019,10 @@
         <f>(0.032114 + 0.017049 + 0.015367)/3</f>
         <v>2.1510000000000001E-2</v>
       </c>
+      <c r="G3" s="5">
+        <f>(0.005371+0.002516+0.005807)/3</f>
+        <v>4.5646666666666665E-3</v>
+      </c>
       <c r="H3" s="2">
         <f>(0.005196+0.005353+0.007827)/3</f>
         <v>6.1253333333333333E-3</v>
@@ -18033,6 +18052,7 @@
         <f>(0.025146 + 0.031812 + 0.026544)/3</f>
         <v>2.7834000000000001E-2</v>
       </c>
+      <c r="G4" s="5"/>
       <c r="H4" s="2">
         <f>(0.015147+0.012408+0.016693)/3</f>
         <v>1.4749333333333335E-2</v>
@@ -18062,6 +18082,7 @@
         <f>(0.077793 + 0.082077 + 0.042202)/3</f>
         <v>6.7357333333333338E-2</v>
       </c>
+      <c r="G5" s="5"/>
       <c r="H5" s="2">
         <f>(0.020408+0.022819+0.018321)/3</f>
         <v>2.0516000000000003E-2</v>
@@ -18091,6 +18112,7 @@
         <f>(0.081262 + 0.065537 + 0.065712)/3</f>
         <v>7.0836999999999997E-2</v>
       </c>
+      <c r="G6" s="5"/>
       <c r="H6" s="2">
         <f>(0.022816 + 0.024383 + 0.023301)/3</f>
         <v>2.3499999999999997E-2</v>
@@ -18118,7 +18140,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
new data graphics values
</commit_message>
<xml_diff>
--- a/files/Rev00_DataGraphics_PTBR.xlsx
+++ b/files/Rev00_DataGraphics_PTBR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/19e359efc7a6f442/Desktop/Enari/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="388" documentId="8_{AECF5A1F-C523-497A-B2A1-66620ACB315E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1477AA46-2FAA-4F8F-A6EC-41BB7A1D21A8}"/>
+  <xr:revisionPtr revIDLastSave="403" documentId="8_{AECF5A1F-C523-497A-B2A1-66620ACB315E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B48299BB-2534-48F0-9292-D234178176EC}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{17A1DBDD-B353-481C-9E41-6E9A6A8B360B}"/>
   </bookViews>
@@ -198,7 +198,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="12">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.00000"/>
     </dxf>
@@ -4022,21 +4025,6 @@
               <c:numCache>
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>7.1536666666666667E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.1510000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.7834000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.7357333333333338E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.0836999999999997E-2</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -5791,6 +5779,21 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -5870,6 +5873,21 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -17006,7 +17024,7 @@
   <autoFilter ref="A1:I6" xr:uid="{A40AA6AD-2F47-43F1-B765-C68DAECD3079}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{7BB7217C-59F8-4792-9EA0-0720D6D8B12E}" name="Tamanho"/>
-    <tableColumn id="2" xr3:uid="{C5127529-A4E4-4639-A4FA-738598E99596}" name="BubbleSort" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{C5127529-A4E4-4639-A4FA-738598E99596}" name="BubbleSort" dataDxfId="11"/>
     <tableColumn id="3" xr3:uid="{D3407327-A185-4351-A55C-14014B1B867D}" name="InsertionSort"/>
     <tableColumn id="4" xr3:uid="{85C71698-96C8-48BF-9E4F-A31F4588E93A}" name="SelectionSort"/>
     <tableColumn id="5" xr3:uid="{D89F0557-14DD-46AD-9565-6B8B49785A1D}" name="MergeSort"/>
@@ -17025,12 +17043,12 @@
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{C1F8DEBA-C1C8-4F0D-B5A8-25CE5185E617}" name="Tamanho"/>
     <tableColumn id="2" xr3:uid="{73836CB1-A1D9-4D27-AA51-8096EC2B23FB}" name="BubbleSort"/>
-    <tableColumn id="3" xr3:uid="{50D01E1E-E49D-48B8-9D64-68BB18FD132D}" name="InsertionSort" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{BF3C1C79-92F0-4E93-AE3F-44D10600C26D}" name="SelectionSort" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{71DF7DE3-1D14-438B-AA85-26258AB0E16E}" name="MergeSort" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{50D01E1E-E49D-48B8-9D64-68BB18FD132D}" name="InsertionSort" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{BF3C1C79-92F0-4E93-AE3F-44D10600C26D}" name="SelectionSort" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{71DF7DE3-1D14-438B-AA85-26258AB0E16E}" name="MergeSort" dataDxfId="8"/>
     <tableColumn id="6" xr3:uid="{D7044A8A-343F-410A-A47C-299C79374E83}" name="QuickSort"/>
-    <tableColumn id="7" xr3:uid="{44EE4653-5828-4AD8-89F5-DCD6FFFB7171}" name="HeapSort" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{06AF528E-0B37-497F-86E3-9CA2A978E533}" name="RadixSort" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{44EE4653-5828-4AD8-89F5-DCD6FFFB7171}" name="HeapSort" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{06AF528E-0B37-497F-86E3-9CA2A978E533}" name="RadixSort" dataDxfId="6"/>
     <tableColumn id="8" xr3:uid="{1AF9EE2E-6E80-48E6-A0EA-B411C6533961}" name="CoutingSort"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -17042,14 +17060,14 @@
   <autoFilter ref="A1:I6" xr:uid="{59E19B13-715F-472A-A7B5-ACE0684BA986}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{88AB9604-3310-46A1-AD70-21C2608B01C8}" name="Tamanho"/>
-    <tableColumn id="2" xr3:uid="{AB29B0C4-1AC7-48FD-8D3C-13AA6916E031}" name="BubbleSort" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{AB29B0C4-1AC7-48FD-8D3C-13AA6916E031}" name="BubbleSort" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{277890D8-FE28-4EFB-A704-7CA343850008}" name="InsertionSort"/>
-    <tableColumn id="4" xr3:uid="{7B9C2A85-4991-44A3-8EB5-C25296FAD161}" name="SelectionSort" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{4450D16D-D01F-43DF-B8B1-9C2BAE2DFD58}" name="MergeSort" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{7B9C2A85-4991-44A3-8EB5-C25296FAD161}" name="SelectionSort" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{4450D16D-D01F-43DF-B8B1-9C2BAE2DFD58}" name="MergeSort" dataDxfId="3"/>
     <tableColumn id="6" xr3:uid="{8F5D90A6-8E0B-4E1B-8D02-4E5B09ACDCA0}" name="QuickSort"/>
     <tableColumn id="7" xr3:uid="{59D8846C-91B6-4237-BE54-A17E0A509527}" name="HeapSort"/>
-    <tableColumn id="8" xr3:uid="{6B8DE172-995E-41FE-BF4F-C27226F78BC4}" name="RadixSort" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{D222E4FB-3FC2-4727-958D-5584BD8905DB}" name="CoutingSort" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{6B8DE172-995E-41FE-BF4F-C27226F78BC4}" name="RadixSort" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{D222E4FB-3FC2-4727-958D-5584BD8905DB}" name="CoutingSort" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -17063,7 +17081,7 @@
     <tableColumn id="2" xr3:uid="{992F9C0B-6668-4206-8062-5710FE0429D1}" name="BubbleSort"/>
     <tableColumn id="3" xr3:uid="{EFA1803E-44E3-404F-87D9-65CCBEE1A3DE}" name="InsertionSort"/>
     <tableColumn id="4" xr3:uid="{A829DF70-6B9C-49B0-870B-D8A3FCDFF1FC}" name="SelectionSort"/>
-    <tableColumn id="5" xr3:uid="{EECD94D9-E658-432D-87FC-A98B3E2C2645}" name="MergeSort"/>
+    <tableColumn id="5" xr3:uid="{EECD94D9-E658-432D-87FC-A98B3E2C2645}" name="MergeSort" dataDxfId="0"/>
     <tableColumn id="6" xr3:uid="{ACF4646F-3D62-4D2C-AFE7-17C20339F4C3}" name="QuickSort"/>
     <tableColumn id="7" xr3:uid="{0B50FEDD-0752-47C3-ABE3-0D8374A536C0}" name="HeapSort"/>
     <tableColumn id="8" xr3:uid="{C8222E89-0ECB-433B-90A5-CBD88DB6FE41}" name="RadixSort"/>
@@ -17922,7 +17940,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17983,10 +18001,7 @@
         <f>(0.151862+0.138773+0.127074)/3</f>
         <v>0.13923633333333332</v>
       </c>
-      <c r="E2" s="4">
-        <f>(0.006058 + 0.006755 + 0.008648)/3</f>
-        <v>7.1536666666666667E-3</v>
-      </c>
+      <c r="E2" s="4"/>
       <c r="G2" s="5">
         <f>(0.002001+0.003001+0.002331)/3</f>
         <v>2.4443333333333335E-3</v>
@@ -18015,10 +18030,7 @@
         <f>(0.56296+0.569012+0.556048)/3</f>
         <v>0.56267333333333325</v>
       </c>
-      <c r="E3" s="4">
-        <f>(0.032114 + 0.017049 + 0.015367)/3</f>
-        <v>2.1510000000000001E-2</v>
-      </c>
+      <c r="E3" s="4"/>
       <c r="G3" s="5">
         <f>(0.005371+0.002516+0.005807)/3</f>
         <v>4.5646666666666665E-3</v>
@@ -18048,10 +18060,7 @@
         <f>(2.38666+2.29391+2.35436)/3</f>
         <v>2.3449766666666663</v>
       </c>
-      <c r="E4" s="4">
-        <f>(0.025146 + 0.031812 + 0.026544)/3</f>
-        <v>2.7834000000000001E-2</v>
-      </c>
+      <c r="E4" s="4"/>
       <c r="G4" s="5"/>
       <c r="H4" s="2">
         <f>(0.015147+0.012408+0.016693)/3</f>
@@ -18078,10 +18087,7 @@
         <f>(9.47137+9.1157+9.18603)/3</f>
         <v>9.2576999999999998</v>
       </c>
-      <c r="E5" s="4">
-        <f>(0.077793 + 0.082077 + 0.042202)/3</f>
-        <v>6.7357333333333338E-2</v>
-      </c>
+      <c r="E5" s="4"/>
       <c r="G5" s="5"/>
       <c r="H5" s="2">
         <f>(0.020408+0.022819+0.018321)/3</f>
@@ -18108,10 +18114,7 @@
         <f>(14.4914+15.2387+14.2372)/3</f>
         <v>14.655766666666667</v>
       </c>
-      <c r="E6" s="4">
-        <f>(0.081262 + 0.065537 + 0.065712)/3</f>
-        <v>7.0836999999999997E-2</v>
-      </c>
+      <c r="E6" s="4"/>
       <c r="G6" s="5"/>
       <c r="H6" s="2">
         <f>(0.022816 + 0.024383 + 0.023301)/3</f>
@@ -18395,25 +18398,55 @@
       <c r="A2">
         <v>10000</v>
       </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>20000</v>
       </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>40000</v>
       </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>80000</v>
       </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>100000</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -18433,7 +18466,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
General update in the files
</commit_message>
<xml_diff>
--- a/files/Rev00_DataGraphics_PTBR.xlsx
+++ b/files/Rev00_DataGraphics_PTBR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/19e359efc7a6f442/Desktop/Enari/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="464" documentId="8_{AECF5A1F-C523-497A-B2A1-66620ACB315E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F92BFC5B-5578-4BBE-B666-F11DBFC05399}"/>
+  <xr:revisionPtr revIDLastSave="498" documentId="8_{AECF5A1F-C523-497A-B2A1-66620ACB315E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71922F59-0D6A-462E-8AB5-353DA40965E3}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{17A1DBDD-B353-481C-9E41-6E9A6A8B360B}"/>
   </bookViews>
@@ -234,6 +234,14 @@
   </cellStyles>
   <dxfs count="12">
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -265,14 +273,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2887,19 +2887,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2.0309999999999998E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0690000000000001E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.1830000000000001E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0179999999999998E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0109999999999998E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2980,6 +2980,21 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3136,21 +3151,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>4.8163333333333331E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.5051333333333333E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.5155E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.8298666666666663E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.8790666666666658E-2</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3853,19 +3853,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.37533833333333333</c:v>
+                  <c:v>0.38360633333333333</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.5142666666666669</c:v>
+                  <c:v>1.6809333333333332</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.6746633333333323</c:v>
+                  <c:v>6.3064099999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22.592433333333332</c:v>
+                  <c:v>25.381833333333333</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35.15826666666667</c:v>
+                  <c:v>38.306199999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4892,19 +4892,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.33670966666666668</c:v>
+                  <c:v>0.33885300000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.5623633333333331</c:v>
+                  <c:v>1.5815999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.593583333333334</c:v>
+                  <c:v>6.0110533333333338</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22.380733333333335</c:v>
+                  <c:v>24.943566666666666</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35.907533333333333</c:v>
+                  <c:v>38.466466666666669</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -17313,7 +17313,7 @@
   <autoFilter ref="A1:I6" xr:uid="{A40AA6AD-2F47-43F1-B765-C68DAECD3079}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{7BB7217C-59F8-4792-9EA0-0720D6D8B12E}" name="Tamanho"/>
-    <tableColumn id="2" xr3:uid="{C5127529-A4E4-4639-A4FA-738598E99596}" name="BubbleSort" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{C5127529-A4E4-4639-A4FA-738598E99596}" name="BubbleSort" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{D3407327-A185-4351-A55C-14014B1B867D}" name="InsertionSort"/>
     <tableColumn id="4" xr3:uid="{85C71698-96C8-48BF-9E4F-A31F4588E93A}" name="SelectionSort"/>
     <tableColumn id="5" xr3:uid="{D89F0557-14DD-46AD-9565-6B8B49785A1D}" name="MergeSort"/>
@@ -17332,12 +17332,12 @@
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{C1F8DEBA-C1C8-4F0D-B5A8-25CE5185E617}" name="Tamanho"/>
     <tableColumn id="2" xr3:uid="{73836CB1-A1D9-4D27-AA51-8096EC2B23FB}" name="BubbleSort"/>
-    <tableColumn id="3" xr3:uid="{50D01E1E-E49D-48B8-9D64-68BB18FD132D}" name="InsertionSort" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{BF3C1C79-92F0-4E93-AE3F-44D10600C26D}" name="SelectionSort" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{71DF7DE3-1D14-438B-AA85-26258AB0E16E}" name="MergeSort" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{50D01E1E-E49D-48B8-9D64-68BB18FD132D}" name="InsertionSort" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{BF3C1C79-92F0-4E93-AE3F-44D10600C26D}" name="SelectionSort" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{71DF7DE3-1D14-438B-AA85-26258AB0E16E}" name="MergeSort" dataDxfId="9"/>
     <tableColumn id="6" xr3:uid="{D7044A8A-343F-410A-A47C-299C79374E83}" name="QuickSort"/>
-    <tableColumn id="7" xr3:uid="{44EE4653-5828-4AD8-89F5-DCD6FFFB7171}" name="HeapSort" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{06AF528E-0B37-497F-86E3-9CA2A978E533}" name="RadixSort" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{44EE4653-5828-4AD8-89F5-DCD6FFFB7171}" name="HeapSort" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{06AF528E-0B37-497F-86E3-9CA2A978E533}" name="RadixSort" dataDxfId="7"/>
     <tableColumn id="8" xr3:uid="{1AF9EE2E-6E80-48E6-A0EA-B411C6533961}" name="CoutingSort"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -17349,14 +17349,14 @@
   <autoFilter ref="A1:I6" xr:uid="{59E19B13-715F-472A-A7B5-ACE0684BA986}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{88AB9604-3310-46A1-AD70-21C2608B01C8}" name="Tamanho"/>
-    <tableColumn id="2" xr3:uid="{AB29B0C4-1AC7-48FD-8D3C-13AA6916E031}" name="BubbleSort" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{AB29B0C4-1AC7-48FD-8D3C-13AA6916E031}" name="BubbleSort" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{277890D8-FE28-4EFB-A704-7CA343850008}" name="InsertionSort"/>
-    <tableColumn id="4" xr3:uid="{7B9C2A85-4991-44A3-8EB5-C25296FAD161}" name="SelectionSort" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{4450D16D-D01F-43DF-B8B1-9C2BAE2DFD58}" name="MergeSort" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{7B9C2A85-4991-44A3-8EB5-C25296FAD161}" name="SelectionSort" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{4450D16D-D01F-43DF-B8B1-9C2BAE2DFD58}" name="MergeSort" dataDxfId="4"/>
     <tableColumn id="6" xr3:uid="{8F5D90A6-8E0B-4E1B-8D02-4E5B09ACDCA0}" name="QuickSort"/>
     <tableColumn id="7" xr3:uid="{59D8846C-91B6-4237-BE54-A17E0A509527}" name="HeapSort"/>
-    <tableColumn id="8" xr3:uid="{6B8DE172-995E-41FE-BF4F-C27226F78BC4}" name="RadixSort" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{D222E4FB-3FC2-4727-958D-5584BD8905DB}" name="CoutingSort" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{6B8DE172-995E-41FE-BF4F-C27226F78BC4}" name="RadixSort" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{D222E4FB-3FC2-4727-958D-5584BD8905DB}" name="CoutingSort" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -17370,7 +17370,7 @@
     <tableColumn id="2" xr3:uid="{992F9C0B-6668-4206-8062-5710FE0429D1}" name="BubbleSort"/>
     <tableColumn id="3" xr3:uid="{EFA1803E-44E3-404F-87D9-65CCBEE1A3DE}" name="InsertionSort"/>
     <tableColumn id="4" xr3:uid="{A829DF70-6B9C-49B0-870B-D8A3FCDFF1FC}" name="SelectionSort"/>
-    <tableColumn id="5" xr3:uid="{EECD94D9-E658-432D-87FC-A98B3E2C2645}" name="MergeSort" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{EECD94D9-E658-432D-87FC-A98B3E2C2645}" name="MergeSort" dataDxfId="1"/>
     <tableColumn id="6" xr3:uid="{ACF4646F-3D62-4D2C-AFE7-17C20339F4C3}" name="QuickSort"/>
     <tableColumn id="7" xr3:uid="{0B50FEDD-0752-47C3-ABE3-0D8374A536C0}" name="HeapSort"/>
     <tableColumn id="8" xr3:uid="{C8222E89-0ECB-433B-90A5-CBD88DB6FE41}" name="RadixSort"/>
@@ -18186,8 +18186,8 @@
   </sheetPr>
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18236,11 +18236,10 @@
         <v>10000</v>
       </c>
       <c r="B2" s="1">
-        <v>2.0309999999999998E-3</v>
-      </c>
-      <c r="E2">
-        <f>(0.006045+0.004368+0.004036)/3</f>
-        <v>4.8163333333333331E-3</v>
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -18248,11 +18247,10 @@
         <v>20000</v>
       </c>
       <c r="B3" s="1">
-        <v>3.0690000000000001E-3</v>
-      </c>
-      <c r="E3">
-        <f>(0.017115+0.012116+0.015923)/3</f>
-        <v>1.5051333333333333E-2</v>
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -18260,11 +18258,10 @@
         <v>40000</v>
       </c>
       <c r="B4" s="1">
-        <v>5.1830000000000001E-3</v>
-      </c>
-      <c r="E4">
-        <f>(0.025742+0.026481+0.023242)/3</f>
-        <v>2.5155E-2</v>
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -18272,11 +18269,10 @@
         <v>80000</v>
       </c>
       <c r="B5" s="1">
-        <v>2.0179999999999998E-3</v>
-      </c>
-      <c r="E5">
-        <f>(0.049628+0.047307+0.047961)/3</f>
-        <v>4.8298666666666663E-2</v>
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -18284,12 +18280,10 @@
         <v>100000</v>
       </c>
       <c r="B6" s="1">
-        <f>(0.002015+0.002007)/2</f>
-        <v>2.0109999999999998E-3</v>
-      </c>
-      <c r="E6">
-        <f>(0.059528+0.053335+0.063509)/3</f>
-        <v>5.8790666666666658E-2</v>
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -18310,7 +18304,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18360,8 +18354,8 @@
         <v>10000</v>
       </c>
       <c r="B2" s="3">
-        <f>(0.400121 + 0.35489 + 0.371004)/3</f>
-        <v>0.37533833333333333</v>
+        <f>(0.373068+0.367002+0.410749)/3</f>
+        <v>0.38360633333333333</v>
       </c>
       <c r="C2" s="3">
         <f>(0.28909+0.278629+0.290539)/3</f>
@@ -18392,8 +18386,8 @@
         <v>20000</v>
       </c>
       <c r="B3" s="3">
-        <f>(1.59393+1.47473+1.47414)/3</f>
-        <v>1.5142666666666669</v>
+        <f>(1.4979+1.77204+1.77286)/3</f>
+        <v>1.6809333333333332</v>
       </c>
       <c r="C3" s="3">
         <f>(1.2161+1.14851+1.23443)/3</f>
@@ -18425,8 +18419,8 @@
         <v>40000</v>
       </c>
       <c r="B4" s="3">
-        <f>(5.73225 + 5.69743 + 5.59431)/3</f>
-        <v>5.6746633333333323</v>
+        <f>(6.37258+6.40264+6.14401)/3</f>
+        <v>6.3064099999999996</v>
       </c>
       <c r="C4" s="3">
         <f>(4.75831+4.64676+4.58611)/3</f>
@@ -18455,8 +18449,8 @@
         <v>80000</v>
       </c>
       <c r="B5" s="3">
-        <f>(22.6429+22.6126+22.5218)/3</f>
-        <v>22.592433333333332</v>
+        <f>(25.4475+26.1256+24.5724)/3</f>
+        <v>25.381833333333333</v>
       </c>
       <c r="C5" s="3">
         <f>(19.0952+18.4903+18.6158)/3</f>
@@ -18485,8 +18479,8 @@
         <v>100000</v>
       </c>
       <c r="B6" s="3">
-        <f>(35.2107+35.4054+34.8587)/3</f>
-        <v>35.15826666666667</v>
+        <f>(38.7489+38.0342+38.1355)/3</f>
+        <v>38.306199999999997</v>
       </c>
       <c r="C6" s="3">
         <f>(29.7728+28.9981+29.5358)/3</f>
@@ -18527,8 +18521,8 @@
   </sheetPr>
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="X14" sqref="X14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18577,8 +18571,8 @@
         <v>10000</v>
       </c>
       <c r="B2" s="3">
-        <f>(0.325188+0.367946+0.316995)/3</f>
-        <v>0.33670966666666668</v>
+        <f>(0.367784+0.317723+0.331052)/3</f>
+        <v>0.33885300000000002</v>
       </c>
       <c r="C2" s="2">
         <f>(0.133132+0.138554+0.141736)/3</f>
@@ -18606,8 +18600,8 @@
         <v>20000</v>
       </c>
       <c r="B3" s="3">
-        <f>(1.52425+1.63456+1.52828)/3</f>
-        <v>1.5623633333333331</v>
+        <f>(1.3813+1.71049+1.65301)/3</f>
+        <v>1.5815999999999999</v>
       </c>
       <c r="C3" s="2">
         <f>(0.547077+0.553206+0.741043)/3</f>
@@ -18635,8 +18629,8 @@
         <v>40000</v>
       </c>
       <c r="B4" s="3">
-        <f>(5.53739+5.55585+5.68751)/3</f>
-        <v>5.593583333333334</v>
+        <f>(6.06465+5.94132+6.02719)/3</f>
+        <v>6.0110533333333338</v>
       </c>
       <c r="C4" s="2">
         <f>(2.27114+2.26733+2.32981)/3</f>
@@ -18664,8 +18658,8 @@
         <v>80000</v>
       </c>
       <c r="B5" s="3">
-        <f>(22.768+22.2722+22.102)/3</f>
-        <v>22.380733333333335</v>
+        <f>(24.9336+25.1887+24.7084)/3</f>
+        <v>24.943566666666666</v>
       </c>
       <c r="C5">
         <f>(9.1501+9.11789+9.45372)/3</f>
@@ -18693,8 +18687,8 @@
         <v>100000</v>
       </c>
       <c r="B6" s="3">
-        <f>(34.6919+35.3491+37.6816)/3</f>
-        <v>35.907533333333333</v>
+        <f>(38.494+38.1501+38.7553)/3</f>
+        <v>38.466466666666669</v>
       </c>
       <c r="C6">
         <f>(14.2188+14.4099+14.4099)/3</f>

</xml_diff>